<commit_message>
Change config and image
</commit_message>
<xml_diff>
--- a/programming-essentials/config.xlsx
+++ b/programming-essentials/config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joren\Documents\repositories\CanvasCourseScaffolder\folder_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joren\Documents\repositories\canvas-course-scaffolder-with-templates\programming-essentials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BD74EB-D8CA-4C19-8319-0491DC51BF13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE88CF6-70C7-4BB7-A290-084AA94D3EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -129,9 +129,6 @@
     <t>Canvas cursus ID</t>
   </si>
   <si>
-    <t>Joren Synaeve, Joeri Verlooy</t>
-  </si>
-  <si>
     <t>Feedback en begeleiding</t>
   </si>
   <si>
@@ -162,12 +159,6 @@
     <t>Naam OPO</t>
   </si>
   <si>
-    <t>course_image.jpg</t>
-  </si>
-  <si>
-    <t>joeri.verlooy@thomasmore.be,joren.synaeve@thomasmore.be,indy.hendrickx@thomasmore.be,matthias.claessen@thomasmore.be</t>
-  </si>
-  <si>
     <t>01.06</t>
   </si>
   <si>
@@ -268,6 +259,15 @@
   </si>
   <si>
     <t>Toets (indien toets)</t>
+  </si>
+  <si>
+    <t>Canvas tile image.png</t>
+  </si>
+  <si>
+    <t>Joren Synaeve, Joeri Verlooy, Matthias Claessen, Indy Hendrickx</t>
+  </si>
+  <si>
+    <t>joren.synaeve@thomasmore.be,joeri.verlooy@thomasmore.be,matthias.claessen@thomasmore.be,indy.hendrickx@thomasmore.be</t>
   </si>
 </sst>
 </file>
@@ -708,7 +708,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -729,7 +731,7 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -737,7 +739,7 @@
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -745,15 +747,15 @@
         <v>25</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>39</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -827,7 +829,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -844,7 +846,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -891,7 +893,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C3" s="1">
         <v>45116.999305555553</v>
@@ -911,7 +913,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C4" s="1">
         <v>45122.999305555553</v>
@@ -928,7 +930,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C5" s="1">
         <v>45198.999305555553</v>
@@ -945,7 +947,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C6" s="1">
         <v>45198.999305555553</v>
@@ -962,7 +964,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C7" s="1">
         <v>45198.999305555553</v>
@@ -979,7 +981,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C8" s="1"/>
       <c r="G8">
@@ -994,7 +996,7 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C9" s="1"/>
       <c r="G9">
@@ -1009,7 +1011,7 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C10" s="1"/>
       <c r="G10">
@@ -1024,7 +1026,7 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C11" s="1"/>
       <c r="G11">
@@ -1039,7 +1041,7 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -1067,7 +1069,7 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -1081,7 +1083,7 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -1095,7 +1097,7 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -1109,7 +1111,7 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -1123,7 +1125,7 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -1137,7 +1139,7 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -1151,7 +1153,7 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -1165,7 +1167,7 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -1179,7 +1181,7 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -1193,7 +1195,7 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -1239,7 +1241,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1341,7 +1343,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1394,7 +1396,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
         <v>14</v>
@@ -1403,19 +1405,19 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F1" t="s">
         <v>17</v>
       </c>
       <c r="G1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1423,7 +1425,7 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
@@ -1440,7 +1442,7 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1454,13 +1456,13 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1468,18 +1470,18 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G6" t="s">
         <v>4</v>
@@ -1487,10 +1489,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G7" t="s">
         <v>5</v>
@@ -1528,13 +1530,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
         <v>62</v>
-      </c>
-      <c r="C1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1550,46 +1552,46 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>28</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
         <v>30</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
         <v>32</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
         <v>34</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>